<commit_message>
output files outputting correctly
</commit_message>
<xml_diff>
--- a/output/Intermediate_2_2000.xlsx
+++ b/output/Intermediate_2_2000.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,6 +621,167 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>English and Communication</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1634</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>French</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>461</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Mathematics</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4402</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Biology</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1767</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Chemistry</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>630</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Physics</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>451</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Computing</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>229</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Processing updated to all subjects:
	-- Need to be mindful of dropping columns that are not actually
	subjects.
	-- Some subject names have wierd stuff in them such as " marks.
</commit_message>
<xml_diff>
--- a/output/Intermediate_2_2000.xlsx
+++ b/output/Intermediate_2_2000.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,11 +509,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mathematics</t>
+          <t>Gaelic (Learners)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4427</v>
+        <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -532,11 +532,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Biology</t>
+          <t>Gaidhlig</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>775</v>
+        <v>3</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -555,11 +555,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>German</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>588</v>
+        <v>57</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -578,11 +578,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>Italian</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1152</v>
+        <v>14</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -601,11 +601,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Computing</t>
+          <t>Latin</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>534</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -624,15 +624,15 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>English and Communication</t>
+          <t>Spanish</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1634</v>
+        <v>52</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -647,15 +647,15 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>French</t>
+          <t>Accounting and Finance</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>461</v>
+        <v>149</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -674,11 +674,11 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4402</v>
+        <v>4427</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -697,11 +697,11 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1767</v>
+        <v>775</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -716,15 +716,15 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Biotechnology</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>630</v>
+        <v>15</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -739,15 +739,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>Chemistry</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>451</v>
+        <v>588</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -762,21 +762,2475 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>Geology</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>13</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Managing Environmental Resources</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Physics</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1152</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Crop Establishment</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>7</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Fish Husbandry</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>6</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Investigating Fish Rearing Systems</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>6</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Investigating the Natural Environment</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>6</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Livestock Production</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>7</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Classical Studies</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>8</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Economics</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>54</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Geography</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>509</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>History</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>515</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Modern Studies</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>328</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Philosophy</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>14</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Politics</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Psychology</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>26</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Religious, Moral and Philosophical Studies</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>38</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Sociology</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>31</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Administration</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>179</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Business Management</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>323</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Care</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>11</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Care Issues for Society</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>Computing</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B37" t="n">
+        <v>534</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Construction Craft Skills</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>15</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Construction Industry Practice</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>14</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Craft and Design</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>445</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Electronic and Electrical Fundamentals</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>46</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Engineering Craft Skills</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>100</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Graphic Communication</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>457</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Health and Safety in Care Settings</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Home Economics - Fashion and Textile Technology</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Home Economics - Health and Food Technology</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>42</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Home Economics - Lifestyle and Consumer Technology</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>5</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Hospitality - General Operations</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>84</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Hospitality - Practical Cookery</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>350</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Hospitality - Professional Cookery</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>85</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Hospitality - Reception and Accommodation Operations</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Information Systems</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>1286</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Structures</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>5</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Technological Studies</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>172</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Travel and Tourism</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>70</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Woodworking Skills</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>705</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Art and Design</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>258</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Drama</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>57</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Media Studies</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>88</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Music</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>218</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Physical Education</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>1069</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>English and Communication</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>1634</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>French</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>461</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Gaelic (Learners)</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>12</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Gaidhlig</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>4</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>German</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>143</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Italian</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>37</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Latin</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>12</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Spanish</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>168</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Accounting and Finance</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>239</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Mathematics</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>4402</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Biology</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>1767</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Biotechnology</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>27</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Chemistry</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>630</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Geology</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>6</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Managing Environmental Resources</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Physics</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>451</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Crop Establishment</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>2</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Fish Husbandry</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Investigating Fish Rearing Systems</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Investigating the Natural Environment</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>2</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Livestock Production</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>2</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Classical Studies</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>16</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Economics</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>64</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Geography</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>324</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>History</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>591</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Modern Studies</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>508</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Philosophy</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>33</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Politics</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>4</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Psychology</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>92</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Religious, Moral and Philosophical Studies</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>95</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Sociology</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>52</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Administration</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>773</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Business Management</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>470</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Care</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>98</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Care Issues for Society</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>13</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Computing</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
         <v>229</v>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E15" t="inlineStr">
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Construction Craft Skills</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Construction Industry Practice</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Craft and Design</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>67</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Electronic and Electrical Fundamentals</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Engineering Craft Skills</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>10</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Graphic Communication</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>166</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Health and Safety in Care Settings</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>1</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Home Economics - Fashion and Textile Technology</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>10</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Home Economics - Health and Food Technology</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>286</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Home Economics - Lifestyle and Consumer Technology</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>26</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Hospitality - General Operations</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>70</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Hospitality - Practical Cookery</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>1269</v>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Hospitality - Professional Cookery</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>71</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Hospitality - Reception and Accommodation Operations</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>3</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Information Systems</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>741</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Structures</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>1</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Technological Studies</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>10</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Travel and Tourism</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>175</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Woodworking Skills</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>124</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Art and Design</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>337</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Drama</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>100</v>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Media Studies</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>86</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Music</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>247</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Intermediate_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Physical Education</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>303</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E121" t="inlineStr">
         <is>
           <t>Intermediate_2</t>
         </is>

</xml_diff>